<commit_message>
actualizando el event storming
</commit_message>
<xml_diff>
--- a/Clase/Modelado de dominio/Modelo enriquecido/Modelo Requerimientos.xlsx
+++ b/Clase/Modelado de dominio/Modelo enriquecido/Modelo Requerimientos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe\Documents\DOO\Proyecto-Documentacion\Clase\Modelado de dominio\Modelo enriquecido\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59C6409-20FD-44DB-8359-1BB17D57DAEE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D762E1-206C-4BA0-86D1-AA5CAC036859}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" firstSheet="4" activeTab="13" xr2:uid="{6EE69970-202F-4A01-98E0-735742FBEC48}"/>
   </bookViews>
@@ -686,7 +686,7 @@
     <t>Persona-Politica-6</t>
   </si>
   <si>
-    <t>No existe una per</t>
+    <t>No existe una persona con el codigo mandado</t>
   </si>
 </sst>
 </file>
@@ -1089,6 +1089,33 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1134,6 +1161,27 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1142,54 +1190,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1853,72 +1853,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="str">
         <f>'Objetos del dominio'!$A$1&amp;":"</f>
         <v>Objeto de Dominio:</v>
       </c>
-      <c r="B2" s="46" t="str">
+      <c r="B2" s="55" t="str">
         <f>'Objetos del dominio'!$A$9</f>
         <v>Compromiso Financiero</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
     </row>
     <row r="3" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="str">
         <f>'Objetos del dominio'!$B$1&amp;":"</f>
         <v>Descripción:</v>
       </c>
-      <c r="B3" s="46" t="str">
+      <c r="B3" s="55" t="str">
         <f>'Objetos del dominio'!$B$9</f>
         <v>Entidad que representa el compromiso financiero, lo cual correspende a un compromiso financiero al que esta ligado a cierta persona.</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
@@ -2201,10 +2201,10 @@
       <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="54" t="s">
+      <c r="A15" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="65" t="s">
         <v>47</v>
       </c>
       <c r="C15" s="20" t="s">
@@ -2212,8 +2212,8 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="55"/>
-      <c r="B16" s="57"/>
+      <c r="A16" s="64"/>
+      <c r="B16" s="66"/>
       <c r="C16" s="20" t="s">
         <v>56</v>
       </c>
@@ -2288,72 +2288,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="str">
         <f>'Objetos del dominio'!$A$1&amp;":"</f>
         <v>Objeto de Dominio:</v>
       </c>
-      <c r="B2" s="46" t="str">
+      <c r="B2" s="55" t="str">
         <f>'Objetos del dominio'!$A$10</f>
         <v>Tipo de Compromiso Financiero</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
     </row>
     <row r="3" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="str">
         <f>'Objetos del dominio'!$B$1&amp;":"</f>
         <v>Descripción:</v>
       </c>
-      <c r="B3" s="46" t="str">
+      <c r="B3" s="55" t="str">
         <f>'Objetos del dominio'!B10</f>
         <v>Entidad que representa un tipo de compromiso financiero, lo cual corresponde a la categoria a la que pertenece un compromiso financiero determinado.</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
@@ -2638,10 +2638,10 @@
       <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="54" t="s">
+      <c r="A15" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="65" t="s">
         <v>47</v>
       </c>
       <c r="C15" s="20" t="s">
@@ -2649,8 +2649,8 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="55"/>
-      <c r="B16" s="57"/>
+      <c r="A16" s="64"/>
+      <c r="B16" s="66"/>
       <c r="C16" s="20" t="s">
         <v>56</v>
       </c>
@@ -2725,72 +2725,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="str">
         <f>'Objetos del dominio'!$A$1&amp;":"</f>
         <v>Objeto de Dominio:</v>
       </c>
-      <c r="B2" s="46" t="str">
+      <c r="B2" s="55" t="str">
         <f>'Objetos del dominio'!A11</f>
         <v>Mes</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
     </row>
     <row r="3" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="str">
         <f>'Objetos del dominio'!$B$1&amp;":"</f>
         <v>Descripción:</v>
       </c>
-      <c r="B3" s="46" t="str">
+      <c r="B3" s="55" t="str">
         <f>'Objetos del dominio'!$B$11</f>
         <v>Entidad que representa un mes, la cual corresponde a un mes en donde se esta administrando el presupuesto. Por ejemplo en el mes febrero se ha realizado x total de gastos.</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
@@ -3000,10 +3000,10 @@
       <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:17" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="58" t="s">
+      <c r="A13" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="59" t="s">
+      <c r="B13" s="68" t="s">
         <v>47</v>
       </c>
       <c r="C13" s="20" t="s">
@@ -3012,8 +3012,8 @@
       <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="58"/>
-      <c r="B14" s="59"/>
+      <c r="A14" s="67"/>
+      <c r="B14" s="68"/>
       <c r="C14" s="20" t="s">
         <v>56</v>
       </c>
@@ -3091,72 +3091,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="str">
         <f>'Objetos del dominio'!$A$1&amp;":"</f>
         <v>Objeto de Dominio:</v>
       </c>
-      <c r="B2" s="46" t="str">
+      <c r="B2" s="55" t="str">
         <f>'Objetos del dominio'!$A$6</f>
         <v>Año</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
     </row>
     <row r="3" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="str">
         <f>'Objetos del dominio'!$B$1&amp;":"</f>
         <v>Descripción:</v>
       </c>
-      <c r="B3" s="46" t="str">
+      <c r="B3" s="55" t="str">
         <f>'Objetos del dominio'!$B$6</f>
         <v>Entidad que representa un año, la cual corresponde al año vigente en que se va a regir el registro del presupuesto correspondiente.</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
@@ -3366,10 +3366,10 @@
       <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:17" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="58" t="s">
+      <c r="A13" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="59" t="s">
+      <c r="B13" s="68" t="s">
         <v>47</v>
       </c>
       <c r="C13" s="20" t="s">
@@ -3378,8 +3378,8 @@
       <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="58"/>
-      <c r="B14" s="59"/>
+      <c r="A14" s="67"/>
+      <c r="B14" s="68"/>
       <c r="C14" s="20" t="s">
         <v>56</v>
       </c>
@@ -3432,7 +3432,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J20" sqref="A20:XFD20"/>
+      <selection pane="bottomLeft" activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3460,72 +3460,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="str">
         <f>'Objetos del dominio'!$A$1&amp;":"</f>
         <v>Objeto de Dominio:</v>
       </c>
-      <c r="B2" s="46" t="str">
+      <c r="B2" s="55" t="str">
         <f>'Objetos del dominio'!$A$7</f>
         <v>Persona</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
     </row>
     <row r="3" spans="1:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="str">
         <f>'Objetos del dominio'!$B$1&amp;":"</f>
         <v>Descripción:</v>
       </c>
-      <c r="B3" s="46" t="str">
+      <c r="B3" s="55" t="str">
         <f>'Objetos del dominio'!$B$7</f>
         <v>Entidad que representa una persona, lo cual corresponde a la persona encargada de registrar, administrar o ver el el historial del presupuesto.</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
@@ -3807,14 +3807,14 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="76" t="s">
         <v>190</v>
       </c>
-      <c r="B11" s="61"/>
-      <c r="C11" s="62"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="78"/>
     </row>
     <row r="12" spans="1:20" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="70" t="s">
+      <c r="A12" s="49" t="s">
         <v>44</v>
       </c>
       <c r="B12" s="18" t="s">
@@ -3843,140 +3843,140 @@
     </row>
     <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="56" t="s">
         <v>160</v>
       </c>
-      <c r="B16" s="48"/>
-      <c r="C16" s="47" t="s">
+      <c r="B16" s="57"/>
+      <c r="C16" s="56" t="s">
         <v>173</v>
       </c>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47" t="s">
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56" t="s">
         <v>191</v>
       </c>
-      <c r="H16" s="48"/>
-      <c r="I16" s="65" t="s">
+      <c r="H16" s="57"/>
+      <c r="I16" s="45" t="s">
         <v>197</v>
       </c>
-      <c r="J16" s="66" t="s">
+      <c r="J16" s="46" t="s">
         <v>198</v>
       </c>
-      <c r="K16" s="69" t="s">
+      <c r="K16" s="72" t="s">
         <v>200</v>
       </c>
-      <c r="L16" s="69"/>
-      <c r="M16" s="69"/>
+      <c r="L16" s="72"/>
+      <c r="M16" s="72"/>
     </row>
     <row r="17" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="63" t="s">
+      <c r="A17" s="73" t="s">
         <v>164</v>
       </c>
-      <c r="B17" s="64"/>
-      <c r="C17" s="51" t="s">
+      <c r="B17" s="75"/>
+      <c r="C17" s="60" t="s">
         <v>174</v>
       </c>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="63" t="s">
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="H17" s="64"/>
+      <c r="H17" s="75"/>
       <c r="I17" s="41"/>
-      <c r="J17" s="67" t="s">
+      <c r="J17" s="47" t="s">
         <v>199</v>
       </c>
-      <c r="K17" s="63" t="s">
+      <c r="K17" s="73" t="s">
         <v>201</v>
       </c>
-      <c r="L17" s="72"/>
-      <c r="M17" s="64"/>
+      <c r="L17" s="74"/>
+      <c r="M17" s="75"/>
     </row>
     <row r="18" spans="1:13" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="63" t="s">
+      <c r="A18" s="73" t="s">
         <v>163</v>
       </c>
-      <c r="B18" s="64"/>
-      <c r="C18" s="50" t="s">
+      <c r="B18" s="75"/>
+      <c r="C18" s="59" t="s">
         <v>175</v>
       </c>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="49" t="s">
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="H18" s="49"/>
+      <c r="H18" s="58"/>
       <c r="I18" s="41"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="49"/>
-      <c r="L18" s="49"/>
-      <c r="M18" s="49"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="58"/>
     </row>
     <row r="19" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="51" t="s">
+      <c r="A19" s="60" t="s">
         <v>162</v>
       </c>
-      <c r="B19" s="53"/>
-      <c r="C19" s="50" t="s">
+      <c r="B19" s="62"/>
+      <c r="C19" s="59" t="s">
         <v>176</v>
       </c>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="49" t="s">
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="H19" s="49"/>
+      <c r="H19" s="58"/>
       <c r="I19" s="41"/>
-      <c r="J19" s="68"/>
-      <c r="K19" s="49"/>
-      <c r="L19" s="49"/>
-      <c r="M19" s="49"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="58"/>
     </row>
     <row r="20" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="59" t="s">
         <v>161</v>
       </c>
-      <c r="B20" s="50"/>
-      <c r="C20" s="50" t="s">
+      <c r="B20" s="59"/>
+      <c r="C20" s="59" t="s">
         <v>177</v>
       </c>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="49" t="s">
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="58" t="s">
         <v>192</v>
       </c>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49" t="s">
+      <c r="H20" s="58"/>
+      <c r="I20" s="58" t="s">
         <v>206</v>
       </c>
-      <c r="J20" s="77" t="s">
+      <c r="J20" s="52" t="s">
         <v>213</v>
       </c>
-      <c r="K20" s="49" t="s">
+      <c r="K20" s="58" t="s">
         <v>214</v>
       </c>
-      <c r="L20" s="49"/>
-      <c r="M20" s="49"/>
+      <c r="L20" s="58"/>
+      <c r="M20" s="58"/>
     </row>
     <row r="21" spans="1:13" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="50"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="78"/>
-      <c r="K21" s="50"/>
-      <c r="L21" s="50"/>
-      <c r="M21" s="50"/>
+      <c r="A21" s="59"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="59"/>
+      <c r="L21" s="59"/>
+      <c r="M21" s="59"/>
     </row>
     <row r="22" spans="1:13" s="9" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
@@ -3984,100 +3984,85 @@
       <c r="C22" s="10"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="71" t="s">
+      <c r="A25" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="73" t="s">
+      <c r="B25" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="74"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="71"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="75" t="s">
+      <c r="A26" s="51" t="s">
         <v>199</v>
       </c>
-      <c r="B26" s="76" t="s">
+      <c r="B26" s="69" t="s">
         <v>202</v>
       </c>
-      <c r="C26" s="76"/>
-      <c r="D26" s="76"/>
-      <c r="E26" s="76"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="75" t="s">
+      <c r="A27" s="51" t="s">
         <v>203</v>
       </c>
-      <c r="B27" s="76" t="s">
+      <c r="B27" s="69" t="s">
         <v>205</v>
       </c>
-      <c r="C27" s="76"/>
-      <c r="D27" s="76"/>
-      <c r="E27" s="76"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="75" t="s">
+      <c r="A28" s="51" t="s">
         <v>204</v>
       </c>
-      <c r="B28" s="76" t="s">
+      <c r="B28" s="69" t="s">
         <v>209</v>
       </c>
-      <c r="C28" s="76"/>
-      <c r="D28" s="76"/>
-      <c r="E28" s="76"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="75" t="s">
+      <c r="A29" s="51" t="s">
         <v>207</v>
       </c>
-      <c r="B29" s="76" t="s">
+      <c r="B29" s="69" t="s">
         <v>210</v>
       </c>
-      <c r="C29" s="76"/>
-      <c r="D29" s="76"/>
-      <c r="E29" s="76"/>
+      <c r="C29" s="69"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="69"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="75" t="s">
+      <c r="A30" s="51" t="s">
         <v>208</v>
       </c>
-      <c r="B30" s="76" t="s">
+      <c r="B30" s="69" t="s">
         <v>211</v>
       </c>
-      <c r="C30" s="76"/>
-      <c r="D30" s="76"/>
-      <c r="E30" s="76"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="75" t="s">
+      <c r="A31" s="51" t="s">
         <v>213</v>
       </c>
-      <c r="B31" s="76" t="s">
+      <c r="B31" s="69" t="s">
         <v>212</v>
       </c>
-      <c r="C31" s="76"/>
-      <c r="D31" s="76"/>
-      <c r="E31" s="76"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="A20:B21"/>
-    <mergeCell ref="C20:F21"/>
-    <mergeCell ref="G20:H21"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="G18:H18"/>
     <mergeCell ref="K21:M21"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="B2:P2"/>
@@ -4094,7 +4079,22 @@
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="C20:F21"/>
+    <mergeCell ref="G20:H21"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos del dominio'!A1" display="Volver al inicio" xr:uid="{8CFF7F28-3055-4D0C-A40E-E6071512BFF6}"/>
@@ -4159,72 +4159,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="str">
         <f>'Objetos del dominio'!$A$1&amp;":"</f>
         <v>Objeto de Dominio:</v>
       </c>
-      <c r="B2" s="46" t="str">
+      <c r="B2" s="55" t="str">
         <f>'Objetos del dominio'!$A$8</f>
         <v>Rol persona</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
     </row>
     <row r="3" spans="1:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="str">
         <f>'Objetos del dominio'!$B$1&amp;":"</f>
         <v>Descripción:</v>
       </c>
-      <c r="B3" s="46" t="str">
+      <c r="B3" s="55" t="str">
         <f>'Objetos del dominio'!$B$8</f>
         <v>Entidad que representa el rol de una persona, lo cual corresponde al tipo de rol que realiza, desempeña una persona en la aplicacion. Por ejemplo una persona que representa a un administrador puede asignar el rol de lector a otros usuarios.</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
@@ -4539,105 +4539,105 @@
       <c r="A15" s="7"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="56" t="s">
         <v>160</v>
       </c>
-      <c r="B16" s="48"/>
-      <c r="C16" s="47" t="s">
+      <c r="B16" s="57"/>
+      <c r="C16" s="56" t="s">
         <v>173</v>
       </c>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47" t="s">
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56" t="s">
         <v>191</v>
       </c>
-      <c r="H16" s="48"/>
+      <c r="H16" s="57"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="63" t="s">
+      <c r="A17" s="73" t="s">
         <v>165</v>
       </c>
-      <c r="B17" s="64"/>
-      <c r="C17" s="50" t="s">
+      <c r="B17" s="75"/>
+      <c r="C17" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="49" t="s">
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="58" t="s">
         <v>195</v>
       </c>
-      <c r="H17" s="49"/>
+      <c r="H17" s="58"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="63" t="s">
+      <c r="A18" s="73" t="s">
         <v>166</v>
       </c>
-      <c r="B18" s="64"/>
-      <c r="C18" s="51" t="s">
+      <c r="B18" s="75"/>
+      <c r="C18" s="60" t="s">
         <v>181</v>
       </c>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="49" t="s">
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="H18" s="49"/>
+      <c r="H18" s="58"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="63" t="s">
+      <c r="A19" s="73" t="s">
         <v>167</v>
       </c>
-      <c r="B19" s="64"/>
-      <c r="C19" s="50" t="s">
+      <c r="B19" s="75"/>
+      <c r="C19" s="59" t="s">
         <v>182</v>
       </c>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="49" t="s">
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="58" t="s">
         <v>196</v>
       </c>
-      <c r="H19" s="49"/>
+      <c r="H19" s="58"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="B20" s="64"/>
-      <c r="C20" s="50" t="s">
+      <c r="B20" s="75"/>
+      <c r="C20" s="59" t="s">
         <v>183</v>
       </c>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="49" t="s">
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="58" t="s">
         <v>195</v>
       </c>
-      <c r="H20" s="49"/>
+      <c r="H20" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="B2:P2"/>
-    <mergeCell ref="B3:P3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="C18:F18"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="B2:P2"/>
+    <mergeCell ref="B3:P3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos del dominio'!A1" display="Volver al inicio" xr:uid="{D93000CF-6B8A-4BA9-ACDC-F8E3A0B36DA6}"/>
@@ -4698,72 +4698,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="str">
         <f>'Objetos del dominio'!$A$1&amp;":"</f>
         <v>Objeto de Dominio:</v>
       </c>
-      <c r="B2" s="46" t="str">
+      <c r="B2" s="55" t="str">
         <f>'Objetos del dominio'!$A$2</f>
         <v>Tipo Rubro</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
     </row>
     <row r="3" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="str">
         <f>'Objetos del dominio'!$B$1&amp;":"</f>
         <v>Descripción:</v>
       </c>
-      <c r="B3" s="46" t="str">
+      <c r="B3" s="55" t="str">
         <f>'Objetos del dominio'!$B$2</f>
         <v>Entidad que representa un tipo de rubro, el cual corresponde a la categoria a la cual pertenece un rubro determinado o un compromiso financiero. Por ejemplo un tipo de rubro puede ser ingreso, el cual indica que los rubros categorizados con el, corresponde a dinero que la persona va a recibir por diferentes razones (salario, inversiones, ganancias ocasionales).</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -5010,10 +5010,10 @@
       <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:17" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="59" t="s">
+      <c r="B14" s="68" t="s">
         <v>47</v>
       </c>
       <c r="C14" s="20" t="s">
@@ -5022,8 +5022,8 @@
       <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="58"/>
-      <c r="B15" s="59"/>
+      <c r="A15" s="67"/>
+      <c r="B15" s="68"/>
       <c r="C15" s="20" t="s">
         <v>56</v>
       </c>
@@ -5085,24 +5085,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="str">
@@ -5179,24 +5179,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="str">
@@ -5479,72 +5479,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="str">
         <f>'Objetos del dominio'!$A$1&amp;":"</f>
         <v>Objeto de Dominio:</v>
       </c>
-      <c r="B2" s="46" t="str">
+      <c r="B2" s="55" t="str">
         <f>'Objetos del dominio'!$A$5</f>
         <v>Detalle Presupuesto</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
     </row>
     <row r="3" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="str">
         <f>'Objetos del dominio'!$B$1&amp;":"</f>
         <v>Descripción:</v>
       </c>
-      <c r="B3" s="46" t="str">
+      <c r="B3" s="55" t="str">
         <f>'Objetos del dominio'!B5</f>
         <v>Entidad que representa un detalle de presupuesto, lo cual corresponde a un detallamiento de un presupuesto determinado. Por ejemplo un detalle de presupuesto es el mes del gasto, la persona implicada, el tipo de gasto, el gasto y el valor gastado.</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
@@ -5875,72 +5875,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="str">
         <f>'Objetos del dominio'!$A$1&amp;":"</f>
         <v>Objeto de Dominio:</v>
       </c>
-      <c r="B2" s="46" t="str">
+      <c r="B2" s="55" t="str">
         <f>'Objetos del dominio'!$A$13</f>
         <v>Ejecucion Real Detalle Presupuesto</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
     </row>
     <row r="3" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="str">
         <f>'Objetos del dominio'!$B$1&amp;":"</f>
         <v>Descripción:</v>
       </c>
-      <c r="B3" s="46" t="str">
+      <c r="B3" s="55" t="str">
         <f>'Objetos del dominio'!$B$13</f>
         <v>Entidad que representa una ejecucion real del detalle del presupuesto, lo cual corresponde a la ejecucion real de un detalle de presupuesto determinado, en otras palabras la ejecucion real detalle de presupuesto es la realizacion final de este detalle de presupuesto.</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
@@ -6272,72 +6272,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="str">
         <f>'Objetos del dominio'!$A$1&amp;":"</f>
         <v>Objeto de Dominio:</v>
       </c>
-      <c r="B2" s="46" t="str">
+      <c r="B2" s="55" t="str">
         <f>'Objetos del dominio'!$A$14</f>
         <v>Historia Detalle de Presupuesto</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
     </row>
     <row r="3" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="str">
         <f>'Objetos del dominio'!$B$1&amp;":"</f>
         <v>Descripción:</v>
       </c>
-      <c r="B3" s="46" t="str">
+      <c r="B3" s="55" t="str">
         <f>'Objetos del dominio'!$B$14</f>
         <v>Entidad que representa una historial del detalle del presupuesto, la cual corresponde a la historia (trazabilidad) que ha tenido un detalle de presupuesto; por ejemplo, una historia de presupuesto presentaria los diferentes movimientos o acciones que se han realizado en un detalle de presupuesto.</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
@@ -6654,63 +6654,58 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="47" t="s">
+      <c r="A17" s="56" t="s">
         <v>160</v>
       </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47" t="s">
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56" t="s">
         <v>173</v>
       </c>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47" t="s">
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="56" t="s">
         <v>191</v>
       </c>
-      <c r="I17" s="48"/>
+      <c r="I17" s="57"/>
     </row>
     <row r="18" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="58" t="s">
         <v>170</v>
       </c>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="50" t="s">
+      <c r="B18" s="58"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="59" t="s">
         <v>178</v>
       </c>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="49" t="s">
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
+      <c r="H18" s="58" t="s">
         <v>193</v>
       </c>
-      <c r="I18" s="49"/>
+      <c r="I18" s="58"/>
     </row>
     <row r="19" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="49" t="s">
+      <c r="A19" s="58" t="s">
         <v>169</v>
       </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="51" t="s">
+      <c r="B19" s="58"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="60" t="s">
         <v>179</v>
       </c>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="49" t="s">
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="58" t="s">
         <v>193</v>
       </c>
-      <c r="I19" s="49"/>
+      <c r="I19" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="B2:P2"/>
-    <mergeCell ref="B3:P3"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="D17:G17"/>
@@ -6718,6 +6713,11 @@
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="B2:P2"/>
+    <mergeCell ref="B3:P3"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos del dominio'!A1" display="Volver al inicio" xr:uid="{FD1F1CAE-4C3D-4742-AA29-D1082BCD5770}"/>
@@ -6778,72 +6778,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="str">
         <f>'Objetos del dominio'!$A$1&amp;":"</f>
         <v>Objeto de Dominio:</v>
       </c>
-      <c r="B2" s="46" t="str">
+      <c r="B2" s="55" t="str">
         <f>'Objetos del dominio'!$A$5</f>
         <v>Detalle Presupuesto</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
     </row>
     <row r="3" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="str">
         <f>'Objetos del dominio'!$B$1&amp;":"</f>
         <v>Descripción:</v>
       </c>
-      <c r="B3" s="46" t="str">
+      <c r="B3" s="55" t="str">
         <f>'Objetos del dominio'!B5</f>
         <v>Entidad que representa un detalle de presupuesto, lo cual corresponde a un detallamiento de un presupuesto determinado. Por ejemplo un detalle de presupuesto es el mes del gasto, la persona implicada, el tipo de gasto, el gasto y el valor gastado.</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
@@ -7245,72 +7245,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="str">
         <f>'Objetos del dominio'!$A$1&amp;":"</f>
         <v>Objeto de Dominio:</v>
       </c>
-      <c r="B2" s="46" t="str">
+      <c r="B2" s="55" t="str">
         <f>'Objetos del dominio'!$A$4</f>
         <v>Presupuesto</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
     </row>
     <row r="3" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="str">
         <f>'Objetos del dominio'!$B$1&amp;":"</f>
         <v>Descripción:</v>
       </c>
-      <c r="B3" s="46" t="str">
+      <c r="B3" s="55" t="str">
         <f>'Objetos del dominio'!$B$4</f>
         <v>Entidad que representa un presupuesto, lo cual corresponde al dinero que se va a administrar.  Por ejemplo un presupuesto puede ser la cantidad determinada de dinero que poseo y pienso cotizar para mis gastos de ocio en el año.</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
@@ -7718,72 +7718,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="str">
         <f>'Objetos del dominio'!$A$1&amp;":"</f>
         <v>Objeto de Dominio:</v>
       </c>
-      <c r="B2" s="46" t="str">
+      <c r="B2" s="55" t="str">
         <f>'Objetos del dominio'!$A$3</f>
         <v>Rubro</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
     </row>
     <row r="3" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="str">
         <f>'Objetos del dominio'!$B$1&amp;":"</f>
         <v>Descripción:</v>
       </c>
-      <c r="B3" s="46" t="str">
+      <c r="B3" s="55" t="str">
         <f>'Objetos del dominio'!$B$3</f>
         <v>Entidad que representa un rubro, el cual corresponde al rubro determinado que representa cada uno de los conceptos en que se divide el presupuesto. Por ejemplo un rubro puede ser  (reparacion, gimnasio, ocio, alimentacion).</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
@@ -8068,7 +8068,7 @@
       <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="54" t="s">
+      <c r="A15" s="63" t="s">
         <v>48</v>
       </c>
       <c r="B15" s="29" t="s">
@@ -8079,7 +8079,7 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="55"/>
+      <c r="A16" s="64"/>
       <c r="B16" s="30"/>
       <c r="C16" s="20" t="s">
         <v>56</v>

</xml_diff>